<commit_message>
Minor changes: Added line of text to Plot_CStorEm_Module.R, changed Sankey harvest to Primary Products = Total Harvest and emphasized that wood/pulp waste was from placing those items in PIU.
</commit_message>
<xml_diff>
--- a/HWP Data/ModelExploration/CA_DiscardEnergyCapture_Test.xlsx
+++ b/HWP Data/ModelExploration/CA_DiscardEnergyCapture_Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\RSTUDIO_GIT_PROJECTS\HWP-C-vR\HWP Data\ExistingData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\RSTUDIO_GIT_PROJECTS\HWP-C-vR\HWP Data\ModelExploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E83A45C-2D6A-4D41-802D-59E179DB22CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8813A5-C5C6-41B4-8170-A32817EE6196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33495" yWindow="1005" windowWidth="24870" windowHeight="15600" tabRatio="767" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="930" windowWidth="28800" windowHeight="15435" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HWP_MODEL_OPTIONS" sheetId="1" r:id="rId1"/>
@@ -1259,7 +1259,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1269,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6306,7 +6306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update v.1.1.  See documentation's new section on this update.  Users can adjust the MC's confidence interval and figures are more flexible at handling longer time intervals of data.
</commit_message>
<xml_diff>
--- a/HWP Data/ModelExploration/CA_DiscardEnergyCapture_Test.xlsx
+++ b/HWP Data/ModelExploration/CA_DiscardEnergyCapture_Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerem\Documents\RSTUDIO_GIT_PROJECTS\HWP-C-vR\HWP Data\ModelExploration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8813A5-C5C6-41B4-8170-A32817EE6196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32863F0-C392-4A8C-A1B2-E12B06B8D5CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="930" windowWidth="28800" windowHeight="15435" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1560" windowWidth="28800" windowHeight="13980" tabRatio="767" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HWP_MODEL_OPTIONS" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="127">
   <si>
     <t>QA_TEST</t>
   </si>
@@ -421,12 +421,15 @@
   <si>
     <t>PIU.PAPER.LOSS</t>
   </si>
+  <si>
+    <t>MC.CI.REPORT</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,6 +563,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -909,9 +918,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -971,9 +981,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1011,7 +1021,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1117,7 +1127,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1259,7 +1269,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1267,15 +1277,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="K1" sqref="K1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>119</v>
       </c>
@@ -1306,20 +1316,23 @@
       <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>8</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>120</v>
       </c>
@@ -1351,15 +1364,18 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="L2">
         <v>0.5</v>
       </c>
       <c r="M2">
+        <v>0.5</v>
+      </c>
+      <c r="N2">
         <v>100</v>
       </c>
-      <c r="N2" t="b">
+      <c r="O2" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>